<commit_message>
Updated TestDataHandler and Added FR64 Test Page
Change-Id: I48a3d34e8941156dbbdbd1dad60bf4fcc785a99c
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Dataset.xlsx
+++ b/src/test/resources/data/Dataset.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IN3Workspace\PaxProtection\src\test\resources\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12090" windowHeight="3675"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="12090" windowHeight="3675"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="15" r:id="rId1"/>
@@ -19,7 +24,6 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -94,9 +98,6 @@
     <t>662,2</t>
   </si>
   <si>
-    <t>FL-ZZ-832-20170818-ALB-LAX-0</t>
-  </si>
-  <si>
     <t>PNR</t>
   </si>
   <si>
@@ -112,9 +113,6 @@
     <t>WUCYFT,KTVTWI,LUTPVB,ETLVPS,KLATWW,CTNVBJ,UXOVNE,LKCYSR,DQUUGH</t>
   </si>
   <si>
-    <t>FL-ZZ-708-20170913-RNO-LAX-0</t>
-  </si>
-  <si>
     <t>All,RNO,LAX</t>
   </si>
   <si>
@@ -197,6 +195,12 @@
   </si>
   <si>
     <t>MaxLateness</t>
+  </si>
+  <si>
+    <t>FL-ZZ-866-20171004-PIT-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-54-20171004-PIE-LAX-0</t>
   </si>
 </sst>
 </file>
@@ -460,28 +464,6 @@
   <dxfs count="12">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -776,11 +758,33 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="10"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -795,16 +799,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G3" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9" dataCellStyle="Hyperlink">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G3" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" dataCellStyle="Hyperlink">
   <autoFilter ref="A1:G3"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="RowSelection" dataDxfId="8"/>
-    <tableColumn id="2" name="URL" dataDxfId="7" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="Disruptions" dataDxfId="6" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" name="PNR" dataDxfId="5" dataCellStyle="Hyperlink"/>
-    <tableColumn id="8" name="PDSFilter" dataDxfId="4" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="PNRFilter" dataDxfId="3" dataCellStyle="Hyperlink"/>
-    <tableColumn id="6" name="Config" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" name="RowSelection" dataDxfId="6"/>
+    <tableColumn id="2" name="URL" dataDxfId="5" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="Disruptions" dataDxfId="4" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="PNR" dataDxfId="3" dataCellStyle="Hyperlink"/>
+    <tableColumn id="8" name="PDSFilter" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="PNRFilter" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" name="Config" dataDxfId="0" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1110,7 +1114,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,65 +1135,65 @@
         <v>0</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>47</v>
-      </c>
       <c r="F2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>48</v>
-      </c>
       <c r="F3" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1203,10 +1207,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:WVN2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1677,10 +1681,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="20">
         <v>502388092</v>
@@ -1703,7 +1707,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,7 +1737,7 @@
     </row>
     <row r="2" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>10</v>
@@ -1742,10 +1746,10 @@
         <v>11</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1778,16 +1782,16 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1828,7 +1832,7 @@
     </row>
     <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>17</v>
@@ -1842,7 +1846,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>18</v>
@@ -1890,48 +1894,48 @@
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="5">
         <v>431733</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1961,15 +1965,15 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="4">
         <v>100</v>

</xml_diff>

<commit_message>
summary drawer test script and new project for new UI
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Dataset.xlsx
+++ b/src/test/resources/data/Dataset.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\PaxProtect\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\PaxProtection\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12090" windowHeight="3675" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="15" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="PDSFilter" sheetId="12" r:id="rId5"/>
     <sheet name="PNRFilter" sheetId="14" r:id="rId6"/>
     <sheet name="Config" sheetId="16" r:id="rId7"/>
+    <sheet name="RWS" sheetId="17" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>URL</t>
   </si>
@@ -204,6 +205,546 @@
   </si>
   <si>
     <t>Gerald0607S</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "tenant": "zz",
+    "state": "ADD",
+    "flightID": "FL-ZZ-6-20171115-ATL-LAX-0",
+    "disruption": {
+      "delay": {
+        "departureDelayMinutes": 69,
+        "arrivalDelayMinutes": 273
+      }
+    },
+    "flightDetails": {
+      "flightNumber": "6",
+      "operationalDate": "2017-11-15",
+      "origin": "AP-ATL",
+      "destination": "AP-LAX",
+      "departureTimeSch": {
+        "$date": "2017-11-15T15:25:00.000Z"
+      },
+      "departureTimeEst": {
+        "$date": "2017-11-15T16:34:00.000Z"
+      },
+      "arrivalTimeSch": {
+        "$date": "2017-11-15T16:35:00.000Z"
+      },
+      "arrivalTimeEst": {
+        "$date": "2017-11-15T21:08:00.000Z"
+      },
+      "firstCompartmentPax": 0,
+      "businessCompartmentPax": 5,
+      "coachCompartmentPax": 109
+    },
+    "terminatingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 5,
+      "coachClassCount": 95,
+      "totalCount": 100
+    },
+    "connectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 14,
+      "totalCount": 14
+    },
+    "misconnectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 14,
+      "totalCount": 14
+    },
+    "totalImpactedPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 5,
+      "coachClassCount": 109,
+      "totalCount": 114
+    }
+  },
+  {
+    "tenant": "zz",
+    "state": "ADD",
+    "flightID": "FL-ZZ-330-20171115-GSP-LAX-0",
+    "disruption": {
+      "delay": {
+        "departureDelayMinutes": 46,
+        "arrivalDelayMinutes": 468
+      }
+    },
+    "flightDetails": {
+      "flightNumber": "330",
+      "operationalDate": "2017-11-15",
+      "origin": "AP-GSP",
+      "destination": "AP-LAX",
+      "departureTimeSch": {
+        "$date": "2017-11-15T19:35:00.000Z"
+      },
+      "departureTimeEst": {
+        "$date": "2017-11-15T20:21:00.000Z"
+      },
+      "arrivalTimeSch": {
+        "$date": "2017-11-15T22:00:00.000Z"
+      },
+      "arrivalTimeEst": {
+        "$date": "2017-11-16T05:48:00.000Z"
+      },
+      "firstCompartmentPax": 0,
+      "businessCompartmentPax": 0,
+      "coachCompartmentPax": 182
+    },
+    "terminatingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 126,
+      "totalCount": 126
+    },
+    "connectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 56,
+      "totalCount": 56
+    },
+    "misconnectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 56,
+      "totalCount": 56
+    },
+    "totalImpactedPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 182,
+      "totalCount": 182
+    }
+  },
+  {
+    "tenant": "zz",
+    "state": "ADD",
+    "flightID": "FL-ZZ-144-20171115-SEA-LAX-0",
+    "disruption": {
+      "delay": {
+        "departureDelayMinutes": 96,
+        "arrivalDelayMinutes": 410
+      }
+    },
+    "flightDetails": {
+      "flightNumber": "144",
+      "operationalDate": "2017-11-15",
+      "origin": "AP-SEA",
+      "destination": "AP-LAX",
+      "departureTimeSch": {
+        "$date": "2017-11-15T20:10:00.000Z"
+      },
+      "departureTimeEst": {
+        "$date": "2017-11-15T21:46:00.000Z"
+      },
+      "arrivalTimeSch": {
+        "$date": "2017-11-15T23:10:00.000Z"
+      },
+      "arrivalTimeEst": {
+        "$date": "2017-11-16T06:00:00.000Z"
+      },
+      "firstCompartmentPax": 0,
+      "businessCompartmentPax": 3,
+      "coachCompartmentPax": 70
+    },
+    "terminatingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 3,
+      "coachClassCount": 47,
+      "totalCount": 50
+    },
+    "connectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 23,
+      "totalCount": 23
+    },
+    "misconnectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 16,
+      "totalCount": 16
+    },
+    "totalImpactedPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 3,
+      "coachClassCount": 70,
+      "totalCount": 73
+    }
+  },
+  {
+    "tenant": "zz",
+    "state": "ADD",
+    "flightID": "FL-ZZ-545-20171115-HRI-LAX-0",
+    "disruption": {
+      "delay": {
+        "departureDelayMinutes": 71,
+        "arrivalDelayMinutes": 443
+      }
+    },
+    "flightDetails": {
+      "flightNumber": "545",
+      "operationalDate": "2017-11-15",
+      "origin": "AP-HRI",
+      "destination": "AP-LAX",
+      "departureTimeSch": {
+        "$date": "2017-11-15T21:50:00.000Z"
+      },
+      "departureTimeEst": {
+        "$date": "2017-11-15T23:01:00.000Z"
+      },
+      "arrivalTimeSch": {
+        "$date": "2017-11-16T02:45:00.000Z"
+      },
+      "arrivalTimeEst": {
+        "$date": "2017-11-16T10:08:00.000Z"
+      },
+      "firstCompartmentPax": 0,
+      "businessCompartmentPax": 0,
+      "coachCompartmentPax": 172
+    },
+    "terminatingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 72,
+      "totalCount": 72
+    },
+    "connectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 100,
+      "totalCount": 100
+    },
+    "misconnectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 96,
+      "totalCount": 96
+    },
+    "totalImpactedPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 172,
+      "totalCount": 172
+    }
+  },
+  {
+    "tenant": "zz",
+    "state": "ADD",
+    "flightID": "FL-ZZ-72-20171115-PIE-LAX-0",
+    "disruption": {
+      "delay": {
+        "departureDelayMinutes": 83,
+        "arrivalDelayMinutes": 501
+      }
+    },
+    "flightDetails": {
+      "flightNumber": "72",
+      "operationalDate": "2017-11-15",
+      "origin": "AP-PIE",
+      "destination": "AP-LAX",
+      "departureTimeSch": {
+        "$date": "2017-11-15T21:40:00.000Z"
+      },
+      "departureTimeEst": {
+        "$date": "2017-11-15T23:03:00.000Z"
+      },
+      "arrivalTimeSch": {
+        "$date": "2017-11-15T23:20:00.000Z"
+      },
+      "arrivalTimeEst": {
+        "$date": "2017-11-16T07:41:00.000Z"
+      },
+      "firstCompartmentPax": 0,
+      "businessCompartmentPax": 1,
+      "coachCompartmentPax": 20
+    },
+    "terminatingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 1,
+      "coachClassCount": 5,
+      "totalCount": 6
+    },
+    "connectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 15,
+      "totalCount": 15
+    },
+    "misconnectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 15,
+      "totalCount": 15
+    },
+    "totalImpactedPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 1,
+      "coachClassCount": 20,
+      "totalCount": 21
+    }
+  },
+  {
+    "tenant": "zz",
+    "state": "ADD",
+    "flightID": "FL-ZZ-860-20171115-JAX-LAX-0",
+    "disruption": {
+      "cancel": {}
+    },
+    "flightDetails": {
+      "flightNumber": "860",
+      "operationalDate": "2017-11-15",
+      "origin": "AP-JAX",
+      "destination": "AP-LAX",
+      "departureTimeSch": {
+        "$date": "2017-11-15T23:10:00.000Z"
+      },
+      "arrivalTimeSch": {
+        "$date": "2017-11-16T01:15:00.000Z"
+      },
+      "firstCompartmentPax": 0,
+      "businessCompartmentPax": 1,
+      "coachCompartmentPax": 65
+    },
+    "terminatingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 1,
+      "coachClassCount": 46,
+      "totalCount": 47
+    },
+    "connectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 19,
+      "totalCount": 19
+    },
+    "misconnectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 0,
+      "totalCount": 0
+    },
+    "totalImpactedPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 1,
+      "coachClassCount": 65,
+      "totalCount": 66
+    }
+  },
+  {
+    "tenant": "zz",
+    "state": "ADD",
+    "flightID": "FL-ZZ-344-20171115-MRI-LAX-0",
+    "disruption": {
+      "cancel": {}
+    },
+    "flightDetails": {
+      "flightNumber": "344",
+      "operationalDate": "2017-11-15",
+      "origin": "AP-MRI",
+      "destination": "AP-LAX",
+      "departureTimeSch": {
+        "$date": "2017-11-15T23:55:00.000Z"
+      },
+      "arrivalTimeSch": {
+        "$date": "2017-11-16T03:25:00.000Z"
+      },
+      "firstCompartmentPax": 0,
+      "businessCompartmentPax": 0,
+      "coachCompartmentPax": 191
+    },
+    "terminatingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 77,
+      "totalCount": 77
+    },
+    "connectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 114,
+      "totalCount": 114
+    },
+    "misconnectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 0,
+      "totalCount": 0
+    },
+    "totalImpactedPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 191,
+      "totalCount": 191
+    }
+  },
+  {
+    "tenant": "zz",
+    "state": "ADD",
+    "flightID": "FL-ZZ-174-20171115-GUM-LAX-0",
+    "disruption": {
+      "delay": {
+        "departureDelayMinutes": 110,
+        "arrivalDelayMinutes": 706
+      }
+    },
+    "flightDetails": {
+      "flightNumber": "174",
+      "operationalDate": "2017-11-15",
+      "origin": "AP-GUM",
+      "destination": "AP-LAX",
+      "departureTimeSch": {
+        "$date": "2017-11-15T22:45:00.000Z"
+      },
+      "departureTimeEst": {
+        "$date": "2017-11-16T00:35:00.000Z"
+      },
+      "arrivalTimeSch": {
+        "$date": "2017-11-16T02:25:00.000Z"
+      },
+      "arrivalTimeEst": {
+        "$date": "2017-11-16T14:11:00.000Z"
+      },
+      "firstCompartmentPax": 0,
+      "businessCompartmentPax": 0,
+      "coachCompartmentPax": 70
+    },
+    "terminatingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 65,
+      "totalCount": 65
+    },
+    "connectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 5,
+      "totalCount": 5
+    },
+    "misconnectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 5,
+      "totalCount": 5
+    },
+    "totalImpactedPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 70,
+      "totalCount": 70
+    }
+  },
+  {
+    "tenant": "zz",
+    "state": "ADD",
+    "flightID": "FL-ZZ-714-20171116-LNA-LAX-0",
+    "disruption": {
+      "cancel": {}
+    },
+    "flightDetails": {
+      "flightNumber": "714",
+      "operationalDate": "2017-11-16",
+      "origin": "AP-LNA",
+      "destination": "AP-LAX",
+      "departureTimeSch": {
+        "$date": "2017-11-16T00:40:00.000Z"
+      },
+      "arrivalTimeSch": {
+        "$date": "2017-11-16T04:00:00.000Z"
+      },
+      "firstCompartmentPax": 0,
+      "businessCompartmentPax": 0,
+      "coachCompartmentPax": 74
+    },
+    "terminatingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 52,
+      "totalCount": 52
+    },
+    "connectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 22,
+      "totalCount": 22
+    },
+    "misconnectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 0,
+      "totalCount": 0
+    },
+    "totalImpactedPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 74,
+      "totalCount": 74
+    }
+  },
+  {
+    "tenant": "zz",
+    "state": "ADD",
+    "flightID": "FL-ZZ-730-20171116-KOA-LAX-0",
+    "disruption": {
+      "cancel": {}
+    },
+    "flightDetails": {
+      "flightNumber": "730",
+      "operationalDate": "2017-11-16",
+      "origin": "AP-KOA",
+      "destination": "AP-LAX",
+      "departureTimeSch": {
+        "$date": "2017-11-16T01:20:00.000Z"
+      },
+      "arrivalTimeSch": {
+        "$date": "2017-11-16T06:55:00.000Z"
+      },
+      "firstCompartmentPax": 0,
+      "businessCompartmentPax": 5,
+      "coachCompartmentPax": 127
+    },
+    "terminatingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 5,
+      "coachClassCount": 117,
+      "totalCount": 122
+    },
+    "connectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 10,
+      "totalCount": 10
+    },
+    "misconnectingPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 0,
+      "coachClassCount": 0,
+      "totalCount": 0
+    },
+    "totalImpactedPax": {
+      "firstClassCount": 0,
+      "businessClassCount": 5,
+      "coachClassCount": 127,
+      "totalCount": 132
+    }
+  }
+]</t>
+  </si>
+  <si>
+    <t>ReflowWorkflowResponseJson</t>
+  </si>
+  <si>
+    <t>Data0</t>
+  </si>
+  <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>[{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-724-20171120-HLN-LAX-0","disruption":{"delay":{"departureDelayMinutes":83,"arrivalDelayMinutes":279}},"flightDetails":{"flightNumber":"724","operationalDate":"2017-11-20","origin":"AP-HLN","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T12:20:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T13:43:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T17:00:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-20T21:39:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":1,"coachCompartmentPax":105},"terminatingPax":{"firstClassCount":0,"businessClassCount":1,"coachClassCount":66,"totalCount":67},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":39,"totalCount":39},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":28,"totalCount":28},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":1,"coachClassCount":105,"totalCount":106}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-716-20171120-BUF-LAX-0","disruption":{"delay":{"departureDelayMinutes":99,"arrivalDelayMinutes":479}},"flightDetails":{"flightNumber":"716","operationalDate":"2017-11-20","origin":"AP-BUF","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T12:15:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T13:54:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T15:25:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-20T23:24:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":92},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":81,"totalCount":81},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":11,"totalCount":11},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":6,"totalCount":6},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":92,"totalCount":92}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-886-20171120-SDF-LAX-0","disruption":{"delay":{"departureDelayMinutes":50,"arrivalDelayMinutes":628}},"flightDetails":{"flightNumber":"886","operationalDate":"2017-11-20","origin":"AP-SDF","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T13:30:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T14:20:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T15:40:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-21T02:08:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":3,"coachCompartmentPax":76},"terminatingPax":{"firstClassCount":0,"businessClassCount":3,"coachClassCount":35,"totalCount":38},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":41,"totalCount":41},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":38,"totalCount":38},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":3,"coachClassCount":76,"totalCount":79}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-712-20171120-LNA-LAX-0","disruption":{"delay":{"departureDelayMinutes":119,"arrivalDelayMinutes":572}},"flightDetails":{"flightNumber":"712","operationalDate":"2017-11-20","origin":"AP-LNA","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T12:40:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T14:39:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T16:00:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-21T01:32:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":7,"coachCompartmentPax":109},"terminatingPax":{"firstClassCount":0,"businessClassCount":7,"coachClassCount":96,"totalCount":103},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":13,"totalCount":13},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":11,"totalCount":11},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":7,"coachClassCount":109,"totalCount":116}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-586-20171120-SJU-LAX-0","disruption":{"delay":{"departureDelayMinutes":42,"arrivalDelayMinutes":652}},"flightDetails":{"flightNumber":"586","operationalDate":"2017-11-20","origin":"AP-SJU","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T15:25:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T16:07:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T21:15:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-21T08:07:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":189},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":51,"totalCount":51},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":138,"totalCount":138},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":131,"totalCount":131},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":189,"totalCount":189}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-574-20171120-PWM-LAX-0","disruption":{"cancel":{}},"flightDetails":{"flightNumber":"574","operationalDate":"2017-11-20","origin":"AP-PWM","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T17:00:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T22:25:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":10,"coachCompartmentPax":72},"terminatingPax":{"firstClassCount":0,"businessClassCount":10,"coachClassCount":0,"totalCount":10},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":72,"totalCount":72},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":10,"coachClassCount":72,"totalCount":82}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-648-20171120-JFK-LAX-0","disruption":{"delay":{"departureDelayMinutes":97,"arrivalDelayMinutes":578}},"flightDetails":{"flightNumber":"648","operationalDate":"2017-11-20","origin":"AP-JFK","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T17:45:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T19:22:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T22:05:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-21T07:43:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":190},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":135,"totalCount":135},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":55,"totalCount":55},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":55,"totalCount":55},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":190,"totalCount":190}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-330-20171120-GSP-LAX-0","disruption":{"cancel":{}},"flightDetails":{"flightNumber":"330","operationalDate":"2017-11-20","origin":"AP-GSP","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T19:35:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T22:00:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":182},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":126,"totalCount":126},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":56,"totalCount":56},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":182,"totalCount":182}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-555-20171120-SNA-LAX-0","disruption":{"cancel":{}},"flightDetails":{"flightNumber":"555","operationalDate":"2017-11-20","origin":"AP-SNA","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T19:40:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-21T00:40:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":10,"coachCompartmentPax":163},"terminatingPax":{"firstClassCount":0,"businessClassCount":4,"coachClassCount":29,"totalCount":33},"connectingPax":{"firstClassCount":0,"businessClassCount":6,"coachClassCount":134,"totalCount":140},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":10,"coachClassCount":163,"totalCount":173}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-340-20171120-GGW-LAX-0","disruption":{"cancel":{}},"flightDetails":{"flightNumber":"340","operationalDate":"2017-11-20","origin":"AP-GGW","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T20:40:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-21T00:05:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":180},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":180,"totalCount":180},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":180,"totalCount":180}}]</t>
   </si>
 </sst>
 </file>
@@ -382,7 +923,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -460,6 +1001,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1217,7 +1761,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1728,8 +2272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,7 +2329,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1890,7 +2434,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2008,4 +2552,51 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
12/05/2017 CHANGES: Page Objects: - PDSListViewPage - PaxImpactPage > Filter, Headers, Solve button
Test Page:
- Sprint 24 > US137580_ListView.java

- Dataset 
- TestDataHandler
- pom.xml

Change-Id: I2ea3b7f075280ca345df1472b0eb4469e96f43ff
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Dataset.xlsx
+++ b/src/test/resources/data/Dataset.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\PaxProtection\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\PaxProtect\PaxProtect\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="15" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="97">
   <si>
     <t>URL</t>
   </si>
@@ -48,27 +48,9 @@
     <t>Password</t>
   </si>
   <si>
-    <t>DisruptionList</t>
-  </si>
-  <si>
-    <t>DisruptedFlight</t>
-  </si>
-  <si>
     <t>PNRList</t>
   </si>
   <si>
-    <t>Resolve</t>
-  </si>
-  <si>
-    <t>MultipleDisruptedFlights</t>
-  </si>
-  <si>
-    <t>FL-ZZ-324-20170714-MRI-LAX-0,FL-ZZ-848-20170714-JRA-LAX-0,FL-ZZ-216-20170714-SLC-LAX-0,FL-ZZ-272-20170714-UDG-LAX-0,FL-ZZ-634-20170714-MYR-LAX-0,FL-ZZ-4-20170714-ATL-LAX-0,FL-ZZ-728-20170714-KOA-LAX-0,FL-ZZ-834-20170714-ALB-LAX-0,FL-ZZ-262-20170714-ELP-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-272-20170714-UDG-LAX-0,FL-ZZ-634-20170714-MYR-LAX-0,FL-ZZ-4-20170714-ATL-LAX-0,FL-ZZ-728-20170714-KOA-LAX-0,FL-ZZ-834-20170714-ALB-LAX-0,FL-ZZ-262-20170714-ELP-LAX-0</t>
-  </si>
-  <si>
     <t>Origin</t>
   </si>
   <si>
@@ -190,12 +172,6 @@
   </si>
   <si>
     <t>MaxLateness</t>
-  </si>
-  <si>
-    <t>FL-ZZ-866-20171004-PIT-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-54-20171004-PIE-LAX-0</t>
   </si>
   <si>
     <t xml:space="preserve">https://pax-protect-ui-shell.run.aws-usw02-pr.ice.predix.io </t>
@@ -746,12 +722,141 @@
   <si>
     <t>[{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-724-20171120-HLN-LAX-0","disruption":{"delay":{"departureDelayMinutes":83,"arrivalDelayMinutes":279}},"flightDetails":{"flightNumber":"724","operationalDate":"2017-11-20","origin":"AP-HLN","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T12:20:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T13:43:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T17:00:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-20T21:39:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":1,"coachCompartmentPax":105},"terminatingPax":{"firstClassCount":0,"businessClassCount":1,"coachClassCount":66,"totalCount":67},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":39,"totalCount":39},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":28,"totalCount":28},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":1,"coachClassCount":105,"totalCount":106}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-716-20171120-BUF-LAX-0","disruption":{"delay":{"departureDelayMinutes":99,"arrivalDelayMinutes":479}},"flightDetails":{"flightNumber":"716","operationalDate":"2017-11-20","origin":"AP-BUF","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T12:15:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T13:54:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T15:25:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-20T23:24:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":92},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":81,"totalCount":81},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":11,"totalCount":11},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":6,"totalCount":6},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":92,"totalCount":92}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-886-20171120-SDF-LAX-0","disruption":{"delay":{"departureDelayMinutes":50,"arrivalDelayMinutes":628}},"flightDetails":{"flightNumber":"886","operationalDate":"2017-11-20","origin":"AP-SDF","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T13:30:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T14:20:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T15:40:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-21T02:08:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":3,"coachCompartmentPax":76},"terminatingPax":{"firstClassCount":0,"businessClassCount":3,"coachClassCount":35,"totalCount":38},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":41,"totalCount":41},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":38,"totalCount":38},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":3,"coachClassCount":76,"totalCount":79}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-712-20171120-LNA-LAX-0","disruption":{"delay":{"departureDelayMinutes":119,"arrivalDelayMinutes":572}},"flightDetails":{"flightNumber":"712","operationalDate":"2017-11-20","origin":"AP-LNA","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T12:40:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T14:39:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T16:00:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-21T01:32:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":7,"coachCompartmentPax":109},"terminatingPax":{"firstClassCount":0,"businessClassCount":7,"coachClassCount":96,"totalCount":103},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":13,"totalCount":13},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":11,"totalCount":11},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":7,"coachClassCount":109,"totalCount":116}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-586-20171120-SJU-LAX-0","disruption":{"delay":{"departureDelayMinutes":42,"arrivalDelayMinutes":652}},"flightDetails":{"flightNumber":"586","operationalDate":"2017-11-20","origin":"AP-SJU","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T15:25:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T16:07:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T21:15:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-21T08:07:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":189},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":51,"totalCount":51},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":138,"totalCount":138},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":131,"totalCount":131},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":189,"totalCount":189}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-574-20171120-PWM-LAX-0","disruption":{"cancel":{}},"flightDetails":{"flightNumber":"574","operationalDate":"2017-11-20","origin":"AP-PWM","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T17:00:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T22:25:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":10,"coachCompartmentPax":72},"terminatingPax":{"firstClassCount":0,"businessClassCount":10,"coachClassCount":0,"totalCount":10},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":72,"totalCount":72},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":10,"coachClassCount":72,"totalCount":82}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-648-20171120-JFK-LAX-0","disruption":{"delay":{"departureDelayMinutes":97,"arrivalDelayMinutes":578}},"flightDetails":{"flightNumber":"648","operationalDate":"2017-11-20","origin":"AP-JFK","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T17:45:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T19:22:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T22:05:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-21T07:43:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":190},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":135,"totalCount":135},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":55,"totalCount":55},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":55,"totalCount":55},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":190,"totalCount":190}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-330-20171120-GSP-LAX-0","disruption":{"cancel":{}},"flightDetails":{"flightNumber":"330","operationalDate":"2017-11-20","origin":"AP-GSP","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T19:35:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T22:00:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":182},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":126,"totalCount":126},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":56,"totalCount":56},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":182,"totalCount":182}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-555-20171120-SNA-LAX-0","disruption":{"cancel":{}},"flightDetails":{"flightNumber":"555","operationalDate":"2017-11-20","origin":"AP-SNA","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T19:40:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-21T00:40:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":10,"coachCompartmentPax":163},"terminatingPax":{"firstClassCount":0,"businessClassCount":4,"coachClassCount":29,"totalCount":33},"connectingPax":{"firstClassCount":0,"businessClassCount":6,"coachClassCount":134,"totalCount":140},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":10,"coachClassCount":163,"totalCount":173}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-340-20171120-GGW-LAX-0","disruption":{"cancel":{}},"flightDetails":{"flightNumber":"340","operationalDate":"2017-11-20","origin":"AP-GGW","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T20:40:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-21T00:05:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":180},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":180,"totalCount":180},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":180,"totalCount":180}}]</t>
   </si>
+  <si>
+    <t>Coldplay00AHFOD</t>
+  </si>
+  <si>
+    <t>FlightNumber</t>
+  </si>
+  <si>
+    <t>Disruptions2</t>
+  </si>
+  <si>
+    <t>Disruptions3</t>
+  </si>
+  <si>
+    <t>Disruptions4</t>
+  </si>
+  <si>
+    <t>DataSet2</t>
+  </si>
+  <si>
+    <t>DataSet3</t>
+  </si>
+  <si>
+    <t>DataSet4</t>
+  </si>
+  <si>
+    <t>DataSet5</t>
+  </si>
+  <si>
+    <t>Disruptions5</t>
+  </si>
+  <si>
+    <t>LoginUser2</t>
+  </si>
+  <si>
+    <t>LoginUser3</t>
+  </si>
+  <si>
+    <t>LoginUser4</t>
+  </si>
+  <si>
+    <t>LoginUser5</t>
+  </si>
+  <si>
+    <t>PNR2</t>
+  </si>
+  <si>
+    <t>PNR3</t>
+  </si>
+  <si>
+    <t>PNR4</t>
+  </si>
+  <si>
+    <t>PNR5</t>
+  </si>
+  <si>
+    <t>PDSFilter2</t>
+  </si>
+  <si>
+    <t>PDSFilter3</t>
+  </si>
+  <si>
+    <t>PDSFilter4</t>
+  </si>
+  <si>
+    <t>PDSFilter5</t>
+  </si>
+  <si>
+    <t>PNRFilter2</t>
+  </si>
+  <si>
+    <t>PNRFilter3</t>
+  </si>
+  <si>
+    <t>PNRFilter4</t>
+  </si>
+  <si>
+    <t>PNRFilter5</t>
+  </si>
+  <si>
+    <t>Config2</t>
+  </si>
+  <si>
+    <t>Config3</t>
+  </si>
+  <si>
+    <t>Config4</t>
+  </si>
+  <si>
+    <t>Config5</t>
+  </si>
+  <si>
+    <t>FL-ZZ-798-20171205-RND-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-736-20171205-MIA-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-786-20171205-STL-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-620-20171205-PBI-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-648-20171205-JFK-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-330-20171205-GSP-LAX-0</t>
+  </si>
+  <si>
+    <t>FlightSortDesc</t>
+  </si>
+  <si>
+    <t>FlightSortNewAsc</t>
+  </si>
+  <si>
+    <t>FlightSortAsc</t>
+  </si>
+  <si>
+    <t>FL-ZZ-144-20171205-SEA-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-545-20171205-HRI-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-555-20171205-SNA-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-60-20171205-PIE-LAX-0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -833,6 +938,13 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -923,7 +1035,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -980,9 +1092,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -996,14 +1105,29 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1349,8 +1473,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G3" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" dataCellStyle="Hyperlink">
-  <autoFilter ref="A1:G3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G7" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" dataCellStyle="Hyperlink">
+  <autoFilter ref="A1:G7"/>
   <tableColumns count="7">
     <tableColumn id="1" name="RowSelection" dataDxfId="6"/>
     <tableColumn id="2" name="URL" dataDxfId="5" dataCellStyle="Hyperlink"/>
@@ -1661,10 +1785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,73 +1801,165 @@
     <col min="7" max="7" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>47</v>
+      <c r="C1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>38</v>
-      </c>
       <c r="D2" s="13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>45</v>
-      </c>
       <c r="G3" s="16" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1760,8 +1976,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1769,7 +1985,7 @@
     <col min="1" max="1" width="14.85546875" style="9" customWidth="1"/>
     <col min="2" max="2" width="58.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="10" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" style="10" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" style="11" customWidth="1"/>
     <col min="7" max="256" width="9.140625" style="8"/>
@@ -2232,30 +2448,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>55</v>
+        <v>27</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>47</v>
       </c>
       <c r="C2" s="19">
         <v>502388092</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>56</v>
+      <c r="D2" s="27" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="26" t="s">
+      <c r="A3" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="30">
+        <v>502702210</v>
+      </c>
+      <c r="D3" s="31" t="s">
         <v>54</v>
-      </c>
-      <c r="C3" s="19">
-        <v>502388092</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2270,17 +2486,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="3" width="43.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
     <col min="5" max="5" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2289,34 +2506,107 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>9</v>
+        <v>32</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>84</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>52</v>
+        <v>93</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>84</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>53</v>
-      </c>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2329,7 +2619,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2345,19 +2635,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
-        <v>41</v>
+      <c r="A2" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2387,41 +2677,41 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2451,57 +2741,57 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D3" s="5">
         <v>431733</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2531,15 +2821,15 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B2" s="4">
         <v>100</v>
@@ -2547,7 +2837,7 @@
       <c r="C2" s="4">
         <v>24</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2573,7 +2863,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -2582,18 +2872,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>57</v>
+        <v>51</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12/18/2017 CHANGES: Page Objects: - PDSGridViewPage - PaxImpactPage > Summary Drawer > 15 60 and 180 mins., and Solve button - PaxImpactPage > Filter > viewOptions - for toggle view Icons
Test Page:
- Sprint 24 > US137581_GridView.java

- Dataset 
- pom.xml

Change-Id: Ibac6676127c5ac8ebd8e6f33f268de235b7cfe92
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Dataset.xlsx
+++ b/src/test/resources/data/Dataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\PaxProtect\PaxProtect\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\PaxProtect_sprint25\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
   <si>
     <t>URL</t>
   </si>
@@ -813,24 +813,6 @@
     <t>Config5</t>
   </si>
   <si>
-    <t>FL-ZZ-798-20171205-RND-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-736-20171205-MIA-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-786-20171205-STL-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-620-20171205-PBI-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-648-20171205-JFK-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-330-20171205-GSP-LAX-0</t>
-  </si>
-  <si>
     <t>FlightSortDesc</t>
   </si>
   <si>
@@ -840,16 +822,37 @@
     <t>FlightSortAsc</t>
   </si>
   <si>
-    <t>FL-ZZ-144-20171205-SEA-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-545-20171205-HRI-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-555-20171205-SNA-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-60-20171205-PIE-LAX-0</t>
+    <t>FL-ZZ-158-20171215-DCA-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-336-20171215-GSP-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-876-20171215-PNM-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-814-20171215-CLT-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-60-20171215-PIE-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-144-20171215-SEA-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-26-20171215-PHL-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-886-20171215-SDF-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-868-20171215-PIT-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-64-20171215-PIE-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-28-20171215-PHL-LAX-0</t>
   </si>
 </sst>
 </file>
@@ -1977,7 +1980,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2489,7 +2492,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,13 +2512,13 @@
         <v>55</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2523,16 +2526,16 @@
         <v>32</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>93</v>
+        <v>87</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>92</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2540,16 +2543,16 @@
         <v>33</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>86</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2557,16 +2560,16 @@
         <v>56</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>93</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2574,16 +2577,16 @@
         <v>57</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>97</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2591,7 +2594,7 @@
         <v>58</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
@@ -2602,7 +2605,7 @@
         <v>63</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>

</xml_diff>

<commit_message>
02/14/2018 CHANGES: Page Objects: - PaxImpactpage.java > Filter - TestDataHandler.java
Test Page:
- Sprint3_18Q1 >  US151900_SearchingInPDS.java

- PaxProtect\src\test\resources\data\Dataset

Change-Id: I8c33184c692803861c9817abab9f5c6a4c21416b
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Dataset.xlsx
+++ b/src/test/resources/data/Dataset.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\PaxProtect_sprint25\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\PaxProtect_18Q1_sprint3\PaxProtect\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="15" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="PNRFilter" sheetId="14" r:id="rId6"/>
     <sheet name="Config" sheetId="16" r:id="rId7"/>
     <sheet name="RWS" sheetId="17" r:id="rId8"/>
+    <sheet name="PDSSearch" sheetId="18" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
   <si>
     <t>URL</t>
   </si>
@@ -723,9 +724,6 @@
     <t>[{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-724-20171120-HLN-LAX-0","disruption":{"delay":{"departureDelayMinutes":83,"arrivalDelayMinutes":279}},"flightDetails":{"flightNumber":"724","operationalDate":"2017-11-20","origin":"AP-HLN","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T12:20:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T13:43:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T17:00:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-20T21:39:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":1,"coachCompartmentPax":105},"terminatingPax":{"firstClassCount":0,"businessClassCount":1,"coachClassCount":66,"totalCount":67},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":39,"totalCount":39},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":28,"totalCount":28},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":1,"coachClassCount":105,"totalCount":106}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-716-20171120-BUF-LAX-0","disruption":{"delay":{"departureDelayMinutes":99,"arrivalDelayMinutes":479}},"flightDetails":{"flightNumber":"716","operationalDate":"2017-11-20","origin":"AP-BUF","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T12:15:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T13:54:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T15:25:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-20T23:24:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":92},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":81,"totalCount":81},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":11,"totalCount":11},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":6,"totalCount":6},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":92,"totalCount":92}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-886-20171120-SDF-LAX-0","disruption":{"delay":{"departureDelayMinutes":50,"arrivalDelayMinutes":628}},"flightDetails":{"flightNumber":"886","operationalDate":"2017-11-20","origin":"AP-SDF","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T13:30:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T14:20:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T15:40:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-21T02:08:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":3,"coachCompartmentPax":76},"terminatingPax":{"firstClassCount":0,"businessClassCount":3,"coachClassCount":35,"totalCount":38},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":41,"totalCount":41},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":38,"totalCount":38},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":3,"coachClassCount":76,"totalCount":79}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-712-20171120-LNA-LAX-0","disruption":{"delay":{"departureDelayMinutes":119,"arrivalDelayMinutes":572}},"flightDetails":{"flightNumber":"712","operationalDate":"2017-11-20","origin":"AP-LNA","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T12:40:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T14:39:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T16:00:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-21T01:32:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":7,"coachCompartmentPax":109},"terminatingPax":{"firstClassCount":0,"businessClassCount":7,"coachClassCount":96,"totalCount":103},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":13,"totalCount":13},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":11,"totalCount":11},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":7,"coachClassCount":109,"totalCount":116}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-586-20171120-SJU-LAX-0","disruption":{"delay":{"departureDelayMinutes":42,"arrivalDelayMinutes":652}},"flightDetails":{"flightNumber":"586","operationalDate":"2017-11-20","origin":"AP-SJU","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T15:25:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T16:07:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T21:15:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-21T08:07:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":189},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":51,"totalCount":51},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":138,"totalCount":138},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":131,"totalCount":131},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":189,"totalCount":189}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-574-20171120-PWM-LAX-0","disruption":{"cancel":{}},"flightDetails":{"flightNumber":"574","operationalDate":"2017-11-20","origin":"AP-PWM","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T17:00:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T22:25:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":10,"coachCompartmentPax":72},"terminatingPax":{"firstClassCount":0,"businessClassCount":10,"coachClassCount":0,"totalCount":10},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":72,"totalCount":72},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":10,"coachClassCount":72,"totalCount":82}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-648-20171120-JFK-LAX-0","disruption":{"delay":{"departureDelayMinutes":97,"arrivalDelayMinutes":578}},"flightDetails":{"flightNumber":"648","operationalDate":"2017-11-20","origin":"AP-JFK","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T17:45:00.000Z"},"departureTimeEst":{"$date":"2017-11-20T19:22:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T22:05:00.000Z"},"arrivalTimeEst":{"$date":"2017-11-21T07:43:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":190},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":135,"totalCount":135},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":55,"totalCount":55},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":55,"totalCount":55},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":190,"totalCount":190}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-330-20171120-GSP-LAX-0","disruption":{"cancel":{}},"flightDetails":{"flightNumber":"330","operationalDate":"2017-11-20","origin":"AP-GSP","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T19:35:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-20T22:00:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":182},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":126,"totalCount":126},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":56,"totalCount":56},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":182,"totalCount":182}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-555-20171120-SNA-LAX-0","disruption":{"cancel":{}},"flightDetails":{"flightNumber":"555","operationalDate":"2017-11-20","origin":"AP-SNA","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T19:40:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-21T00:40:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":10,"coachCompartmentPax":163},"terminatingPax":{"firstClassCount":0,"businessClassCount":4,"coachClassCount":29,"totalCount":33},"connectingPax":{"firstClassCount":0,"businessClassCount":6,"coachClassCount":134,"totalCount":140},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":10,"coachClassCount":163,"totalCount":173}},{"tenant":"zz","state":"ADD","flightID":"FL-ZZ-340-20171120-GGW-LAX-0","disruption":{"cancel":{}},"flightDetails":{"flightNumber":"340","operationalDate":"2017-11-20","origin":"AP-GGW","destination":"AP-LAX","departureTimeSch":{"$date":"2017-11-20T20:40:00.000Z"},"arrivalTimeSch":{"$date":"2017-11-21T00:05:00.000Z"},"firstCompartmentPax":0,"businessCompartmentPax":0,"coachCompartmentPax":180},"terminatingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":180,"totalCount":180},"connectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"misconnectingPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":0,"totalCount":0},"totalImpactedPax":{"firstClassCount":0,"businessClassCount":0,"coachClassCount":180,"totalCount":180}}]</t>
   </si>
   <si>
-    <t>Coldplay00AHFOD</t>
-  </si>
-  <si>
     <t>FlightNumber</t>
   </si>
   <si>
@@ -822,37 +820,67 @@
     <t>FlightSortAsc</t>
   </si>
   <si>
-    <t>FL-ZZ-158-20171215-DCA-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-336-20171215-GSP-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-876-20171215-PNM-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-814-20171215-CLT-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-60-20171215-PIE-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-144-20171215-SEA-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-26-20171215-PHL-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-886-20171215-SDF-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-868-20171215-PIT-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-64-20171215-PIE-LAX-0</t>
-  </si>
-  <si>
-    <t>FL-ZZ-28-20171215-PHL-LAX-0</t>
+    <t>Foster00SHC</t>
+  </si>
+  <si>
+    <t>PDSSearch0</t>
+  </si>
+  <si>
+    <t>PDSSearch1</t>
+  </si>
+  <si>
+    <t>PDSSearch</t>
+  </si>
+  <si>
+    <t>PDSSearch2</t>
+  </si>
+  <si>
+    <t>PDSSearch3</t>
+  </si>
+  <si>
+    <t>PDSSearch4</t>
+  </si>
+  <si>
+    <t>PDSSearch5</t>
+  </si>
+  <si>
+    <t>ImpactType</t>
+  </si>
+  <si>
+    <t>Tail</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>FL-ZZ-52-20180213-PIE-LAX-0</t>
+  </si>
+  <si>
+    <t>zz52</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>F0</t>
+  </si>
+  <si>
+    <t>sweet potato</t>
+  </si>
+  <si>
+    <t>FL-ZZ-64-20180213-PIE-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-728-20180213-KOA-LAX-0</t>
+  </si>
+  <si>
+    <t>PIE</t>
+  </si>
+  <si>
+    <t>FL-ZZ-60-20180213-PIE-LAX-0</t>
+  </si>
+  <si>
+    <t>FL-ZZ-894-20180213-COU-LAX-0</t>
   </si>
 </sst>
 </file>
@@ -985,7 +1013,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1032,13 +1060,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1132,13 +1173,52 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1460,8 +1540,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="11"/>
-      <tableStyleElement type="headerRow" dxfId="10"/>
+      <tableStyleElement type="wholeTable" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1476,16 +1556,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G7" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" dataCellStyle="Hyperlink">
-  <autoFilter ref="A1:G7"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="RowSelection" dataDxfId="6"/>
-    <tableColumn id="2" name="URL" dataDxfId="5" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="Disruptions" dataDxfId="4" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" name="PNR" dataDxfId="3" dataCellStyle="Hyperlink"/>
-    <tableColumn id="8" name="PDSFilter" dataDxfId="2" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="PNRFilter" dataDxfId="1" dataCellStyle="Hyperlink"/>
-    <tableColumn id="6" name="Config" dataDxfId="0" dataCellStyle="Hyperlink"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H7" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8" dataCellStyle="Hyperlink">
+  <autoFilter ref="A1:H7"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="RowSelection" dataDxfId="7"/>
+    <tableColumn id="2" name="URL" dataDxfId="6" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="Disruptions" dataDxfId="5" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="PNR" dataDxfId="4" dataCellStyle="Hyperlink"/>
+    <tableColumn id="8" name="PDSFilter" dataDxfId="3" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="PNRFilter" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" name="Config" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" name="PDSSearch" dataDxfId="0" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1788,10 +1869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,9 +1883,10 @@
     <col min="4" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
@@ -1826,8 +1908,11 @@
       <c r="G1" s="21" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>26</v>
       </c>
@@ -1849,8 +1934,11 @@
       <c r="G2" s="13" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>28</v>
       </c>
@@ -1872,97 +1960,112 @@
       <c r="G3" s="16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B5" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C5" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D5" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E5" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F5" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G5" s="16" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="H5" s="33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B6" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C6" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D6" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E6" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F6" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G6" s="16" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="H6" s="33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B7" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="16" t="s">
+      <c r="C7" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E7" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F7" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G7" s="16" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>83</v>
+      <c r="H7" s="33" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2474,7 +2577,7 @@
         <v>502702210</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2491,8 +2594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,16 +2612,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2526,75 +2629,51 @@
         <v>32</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>91</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>96</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>92</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>94</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
@@ -2602,11 +2681,9 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>93</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B7" s="32"/>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
       <c r="E7" s="4"/>
@@ -2663,7 +2740,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2892,4 +2969,86 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="4">
+        <v>728</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
04/04/2018 CHANGES: Page Objects: - PaxImpactpage.java > Filter - FilteringWindowPage.java
Test Page:
- Sprint6_18Q1 >  DE21617_ClearFunctionInPaxImpactPage.java

Change-Id: I98dcebed9d825d1fdb468284fd9f5db17c5221b8
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Dataset.xlsx
+++ b/src/test/resources/data/Dataset.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\PaxProtect_18Q1_sprint3\PaxProtect\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\PaxProtect_18Q1_sprint6\PaxProtect\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="15" r:id="rId1"/>
@@ -2082,7 +2082,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2975,7 +2975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>